<commit_message>
Upload dos testes de mesa
</commit_message>
<xml_diff>
--- a/atividades_LP1/src/Teste de mesa.xlsx
+++ b/atividades_LP1/src/Teste de mesa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noite\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/164409a74d87f087/Área de Trabalho/FATEC/2º SEM/Linguagem Programação I - Java/GitHub/LP-I_Fatec2023/atividades_LP1/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{707966F2-0BD1-4AD0-802C-A606C773E0E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="8_{707966F2-0BD1-4AD0-802C-A606C773E0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADA7E274-6424-411C-B04B-27245DAB1805}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{02605B0D-6FF8-4CFA-AB40-DA6124946025}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{02605B0D-6FF8-4CFA-AB40-DA6124946025}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
   <si>
     <t>Teste de mesa</t>
   </si>
@@ -169,6 +169,120 @@
   </si>
   <si>
     <t>Legenda</t>
+  </si>
+  <si>
+    <t>Exercício 9</t>
+  </si>
+  <si>
+    <t>salario_atual</t>
+  </si>
+  <si>
+    <t>percentual</t>
+  </si>
+  <si>
+    <t>salario_ajustado</t>
+  </si>
+  <si>
+    <t>(10)</t>
+  </si>
+  <si>
+    <t>(1000)</t>
+  </si>
+  <si>
+    <t>{1100}</t>
+  </si>
+  <si>
+    <t>Exercício 10</t>
+  </si>
+  <si>
+    <t>custo_fabrica</t>
+  </si>
+  <si>
+    <t>distribuidor</t>
+  </si>
+  <si>
+    <t>impostos</t>
+  </si>
+  <si>
+    <t>custo_final</t>
+  </si>
+  <si>
+    <t>(10000)</t>
+  </si>
+  <si>
+    <t>{17300}</t>
+  </si>
+  <si>
+    <t>Exercício 11</t>
+  </si>
+  <si>
+    <t>carros_vendidos</t>
+  </si>
+  <si>
+    <t>vendas</t>
+  </si>
+  <si>
+    <t>salario</t>
+  </si>
+  <si>
+    <t>comissao</t>
+  </si>
+  <si>
+    <t>salario_final</t>
+  </si>
+  <si>
+    <t>(200000)</t>
+  </si>
+  <si>
+    <t>(2000)</t>
+  </si>
+  <si>
+    <t>{22000}</t>
+  </si>
+  <si>
+    <t>Exercício 12</t>
+  </si>
+  <si>
+    <t>temp_fahrenheit</t>
+  </si>
+  <si>
+    <t>temp_celsius</t>
+  </si>
+  <si>
+    <t>(98)</t>
+  </si>
+  <si>
+    <t>36.6</t>
+  </si>
+  <si>
+    <t>{36.6}</t>
+  </si>
+  <si>
+    <t>Exercício 13</t>
+  </si>
+  <si>
+    <t>nota_1</t>
+  </si>
+  <si>
+    <t>nota_2</t>
+  </si>
+  <si>
+    <t>nota_3</t>
+  </si>
+  <si>
+    <t>media_final</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>(9)</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>{7.3}</t>
   </si>
 </sst>
 </file>
@@ -584,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -607,6 +721,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,45 +787,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -673,22 +805,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -709,7 +826,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1005,16 +1122,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72AB5D00-39ED-4A78-8F5F-9194E2EB139F}">
-  <dimension ref="B1:I45"/>
+  <dimension ref="B1:I83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="7"/>
-    <col min="7" max="7" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="7"/>
+    <col min="3" max="3" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="7"/>
@@ -1022,28 +1143,28 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-      <c r="G2" s="8" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="G2" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="G3" s="20" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="G3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1060,96 +1181,96 @@
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="30">
+      <c r="B5" s="21">
         <v>9</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>10</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="30">
+      <c r="B6" s="21">
         <v>10</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
         <v>20</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="30">
+      <c r="B7" s="21">
         <v>12</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="30">
+      <c r="B8" s="21">
         <v>13</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>20</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="31">
+      <c r="B9" s="22">
         <v>14</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10">
         <v>10</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="31">
+      <c r="B10" s="22">
         <v>16</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="32">
+      <c r="B11" s="23">
         <v>17</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -1163,40 +1284,40 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="30">
+      <c r="B15" s="21">
         <v>9</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="31">
+      <c r="B16" s="22">
         <v>12</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="14">
+      <c r="C16" s="15"/>
+      <c r="D16" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="32">
+      <c r="B17" s="23">
         <v>14</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
@@ -1213,56 +1334,56 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="30">
+      <c r="B21" s="21">
         <v>9</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="31">
+      <c r="B22" s="22">
         <v>11</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18" t="s">
+      <c r="C22" s="15"/>
+      <c r="D22" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="31">
+      <c r="B23" s="22">
         <v>14</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14">
+      <c r="C23" s="15"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="32">
+      <c r="B24" s="23">
         <v>16</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -1282,78 +1403,78 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="30">
+      <c r="B28" s="21">
         <v>9</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="12"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="30">
+      <c r="B29" s="21">
         <v>11</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17" t="s">
+      <c r="C29" s="14"/>
+      <c r="D29" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="12"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="30">
+      <c r="B30" s="21">
         <v>13</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="17" t="s">
+      <c r="C30" s="14"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="12"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="30">
+      <c r="B31" s="21">
         <v>15</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12">
+      <c r="C31" s="14"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9">
         <v>7375</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="32">
+      <c r="B32" s="23">
         <v>18</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="16" t="s">
+      <c r="C32" s="16"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="35"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="26"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
@@ -1382,159 +1503,540 @@
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="30">
+      <c r="B36" s="21">
         <v>7</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="9"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="30">
+      <c r="B37" s="21">
         <v>9</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17" t="s">
+      <c r="C37" s="14"/>
+      <c r="D37" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="12"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="9"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="30">
+      <c r="B38" s="21">
         <v>11</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="17" t="s">
+      <c r="C38" s="14"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="12"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="9"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="30">
+      <c r="B39" s="21">
         <v>13</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="17" t="s">
+      <c r="C39" s="14"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="12"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="9"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="30">
+      <c r="B40" s="21">
         <v>19</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11" t="s">
+      <c r="C40" s="14"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="12"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="9"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="30">
+      <c r="B41" s="21">
         <v>20</v>
       </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11">
+      <c r="C41" s="14"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8">
         <v>10</v>
       </c>
-      <c r="I41" s="12"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="30">
+      <c r="B42" s="21">
         <v>21</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="12" t="s">
+      <c r="C42" s="14"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="30">
+      <c r="B43" s="21">
         <v>23</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11" t="s">
+      <c r="C43" s="14"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H43" s="11"/>
-      <c r="I43" s="12"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="9"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="30">
+      <c r="B44" s="21">
         <v>24</v>
       </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11" t="s">
+      <c r="C44" s="14"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I44" s="12"/>
+      <c r="I44" s="9"/>
     </row>
     <row r="45" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="32">
+      <c r="B45" s="23">
         <v>25</v>
       </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="16" t="s">
+      <c r="C45" s="16"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="13" t="s">
         <v>46</v>
       </c>
     </row>
+    <row r="46" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="26"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="21">
+        <v>7</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="21">
+        <v>9</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="9"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="21">
+        <v>13</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="36">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="23">
+        <v>15</v>
+      </c>
+      <c r="C52" s="16"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="26"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="21">
+        <v>7</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="21">
+        <v>13</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14">
+        <v>2800</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="21">
+        <v>14</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="14">
+        <v>4500</v>
+      </c>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="21">
+        <v>16</v>
+      </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="36">
+        <v>17300</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="23">
+        <v>18</v>
+      </c>
+      <c r="C60" s="16"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="26"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="21">
+        <v>7</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="9"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="21">
+        <v>9</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="9"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="21">
+        <v>11</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F66" s="8"/>
+      <c r="G66" s="9"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="21">
+        <v>13</v>
+      </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G67" s="9"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="21">
+        <v>17</v>
+      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="9">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="23">
+        <v>19</v>
+      </c>
+      <c r="C69" s="16"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C71" s="25"/>
+      <c r="D71" s="26"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="21">
+        <v>7</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D73" s="9"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="22">
+        <v>11</v>
+      </c>
+      <c r="C74" s="15"/>
+      <c r="D74" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="23">
+        <v>13</v>
+      </c>
+      <c r="C75" s="16"/>
+      <c r="D75" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" s="25"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="25"/>
+      <c r="F77" s="26"/>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="21">
+        <v>7</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="9"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="21">
+        <v>9</v>
+      </c>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E80" s="8"/>
+      <c r="F80" s="9"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="21">
+        <v>11</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F81" s="9"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="21">
+        <v>15</v>
+      </c>
+      <c r="C82" s="14"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="23">
+        <v>17</v>
+      </c>
+      <c r="C83" s="16"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="12">
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B62:G62"/>
     <mergeCell ref="B34:I34"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B13:D13"/>

</xml_diff>